<commit_message>
Added files, minor changes
</commit_message>
<xml_diff>
--- a/Bill of Materials.xlsx
+++ b/Bill of Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shield Parts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="84">
   <si>
     <t>Number</t>
   </si>
@@ -177,18 +177,6 @@
     <t>http://www.newark.com/te-connectivity/2041021-3/memory-card-connector-sd-9-position/dp/35R2925?CMP=AFC-QO1721829242?gross_price=</t>
   </si>
   <si>
-    <t>Quad Buffer</t>
-  </si>
-  <si>
-    <t>595-SN74AHC125MDREP</t>
-  </si>
-  <si>
-    <t>SOIC-14</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Texas-Instruments/SN74AHC125MDREP/?qs=sGAEpiMZZMuiiWkaIwCK2S7iisUJKLbkCxHZbiEL4Hk%3d</t>
-  </si>
-  <si>
     <t>859-LTST-C170CKT</t>
   </si>
   <si>
@@ -289,6 +277,9 @@
   </si>
   <si>
     <t>http://www.linear.com/product/LT3652</t>
+  </si>
+  <si>
+    <t>Transistor for soil sensors</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1226,7 +1217,7 @@
       <c r="M2" s="50"/>
       <c r="N2" s="51"/>
       <c r="O2" s="46" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1614,13 +1605,13 @@
         <v>24</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="M13" s="29" t="s">
         <v>40</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O13" s="44"/>
     </row>
@@ -1658,13 +1649,13 @@
         <v>24</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>40</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="O14" s="44"/>
     </row>
@@ -1759,52 +1750,34 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="39">
-        <v>1.87</v>
-      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="26">
         <f t="shared" si="3"/>
-        <v>1.87</v>
-      </c>
-      <c r="G17" s="21">
-        <v>1.68</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G17" s="21"/>
       <c r="H17" s="20">
         <f t="shared" si="4"/>
-        <v>16.8</v>
-      </c>
-      <c r="I17" s="21">
-        <v>1.46</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I17" s="21"/>
       <c r="J17" s="20">
         <f t="shared" si="5"/>
-        <v>36.5</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="19" t="s">
-        <v>52</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="19"/>
       <c r="O17" s="44"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1834,23 +1807,23 @@
         <v>24</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O18" s="44" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="34"/>
       <c r="C19" s="25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" s="4">
         <v>1</v>
@@ -1880,23 +1853,23 @@
         <v>24</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M19" s="29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O19" s="44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D20" s="4">
         <v>5</v>
@@ -1926,23 +1899,23 @@
         <v>24</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="O20" s="44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -1972,13 +1945,13 @@
         <v>24</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M21" s="29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O21" s="44"/>
     </row>
@@ -2222,21 +2195,21 @@
       </c>
       <c r="F31" s="24">
         <f>SUM(F4:F30)</f>
-        <v>24.770000000000003</v>
+        <v>22.9</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="24">
         <f t="shared" ref="H31:J31" si="6">SUM(H4:H30)</f>
-        <v>237.66</v>
+        <v>220.85999999999999</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="J31" s="24">
         <f t="shared" si="6"/>
-        <v>557.15</v>
+        <v>520.65</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2245,21 +2218,21 @@
       </c>
       <c r="F32" s="24">
         <f>F31</f>
-        <v>24.770000000000003</v>
+        <v>22.9</v>
       </c>
       <c r="G32" t="s">
         <v>17</v>
       </c>
       <c r="H32" s="35">
         <f>H31/10</f>
-        <v>23.765999999999998</v>
+        <v>22.085999999999999</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="35">
         <f>J31/25</f>
-        <v>22.285999999999998</v>
+        <v>20.826000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2279,7 +2252,7 @@
     <hyperlink ref="N12" r:id="rId4"/>
     <hyperlink ref="N15" r:id="rId5"/>
     <hyperlink ref="N16" r:id="rId6"/>
-    <hyperlink ref="N17" r:id="rId7"/>
+    <hyperlink ref="N18" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2291,7 +2264,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2303,10 +2276,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2314,26 +2287,26 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -2343,12 +2316,17 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2363,7 +2341,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>